<commit_message>
Actualización de la lista de entregables. Echarle un ojo para que ver los entregables que faltan por subir. (K)
</commit_message>
<xml_diff>
--- a/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
+++ b/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esgar\OneDrive\Documentos\Sack-3D\Documentacion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId3"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
   <si>
     <t>Lista de Entregables HITO 1</t>
   </si>
@@ -116,53 +124,97 @@
   </si>
   <si>
     <t>Boceto del entorno</t>
+  </si>
+  <si>
+    <t>Armas</t>
+  </si>
+  <si>
+    <t>Movimiento, salto, hacerse el muerto y disparar</t>
+  </si>
+  <si>
+    <t>Cargador de mapas desde Tiled</t>
+  </si>
+  <si>
+    <t>Muelles y cosas</t>
+  </si>
+  <si>
+    <t>Moviento con los cubos creables</t>
+  </si>
+  <si>
+    <t>Coger y soltar cosas</t>
+  </si>
+  <si>
+    <t>Falta esto</t>
+  </si>
+  <si>
+    <t>Esto no se ni que es</t>
+  </si>
+  <si>
+    <t>Listo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00;[Red]\-0.00;&quot;&quot;"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <sz val="36.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="36"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF4C1900"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="'Helvetica Neue'"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF21FF51"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -170,7 +222,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -209,129 +261,392 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="34">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="6" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF21FF51"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="3" width="14.57"/>
-    <col customWidth="1" min="4" max="4" width="102.57"/>
+    <col min="1" max="1" width="6.21875" customWidth="1"/>
+    <col min="2" max="2" width="39.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="102.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="24.75" customHeight="1">
+    <row r="2" spans="2:9" ht="24.75" customHeight="1">
       <c r="G2" s="1"/>
     </row>
-    <row r="3" ht="62.25" customHeight="1">
+    <row r="3" spans="2:9" ht="62.25" customHeight="1">
       <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
@@ -339,7 +654,7 @@
       <c r="G3" s="4"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4">
+    <row r="4" spans="2:9" ht="15.6">
       <c r="D4" s="6" t="s">
         <v>1</v>
       </c>
@@ -347,11 +662,11 @@
       <c r="G4" s="4"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5">
+    <row r="5" spans="2:9" ht="15.6">
       <c r="G5" s="4"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6">
+    <row r="6" spans="2:9" ht="17.399999999999999">
       <c r="C6" s="7" t="s">
         <v>2</v>
       </c>
@@ -366,7 +681,10 @@
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7">
+    <row r="7" spans="2:9" ht="15.6">
+      <c r="B7" s="32" t="s">
+        <v>41</v>
+      </c>
       <c r="C7" s="8" t="s">
         <v>6</v>
       </c>
@@ -374,7 +692,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="10">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="F7" s="11">
         <v>4.91</v>
@@ -384,7 +702,10 @@
       </c>
       <c r="I7" s="5"/>
     </row>
-    <row r="8">
+    <row r="8" spans="2:9" ht="15">
+      <c r="B8" s="32" t="s">
+        <v>41</v>
+      </c>
       <c r="C8" s="8" t="s">
         <v>6</v>
       </c>
@@ -392,13 +713,16 @@
         <v>9</v>
       </c>
       <c r="E8" s="10">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="F8" s="11">
         <v>3.27</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="2:9" ht="15">
+      <c r="B9" s="32" t="s">
+        <v>41</v>
+      </c>
       <c r="C9" s="8" t="s">
         <v>6</v>
       </c>
@@ -406,14 +730,17 @@
         <v>10</v>
       </c>
       <c r="E9" s="14">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="F9" s="11">
-        <v>2.45</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" spans="2:9" ht="15">
+      <c r="B10" s="33" t="s">
+        <v>43</v>
+      </c>
       <c r="C10" s="8" t="s">
         <v>6</v>
       </c>
@@ -421,14 +748,17 @@
         <v>11</v>
       </c>
       <c r="E10" s="14">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="F10" s="11">
         <v>2.36</v>
       </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11">
+    <row r="11" spans="2:9" ht="15">
+      <c r="B11" s="33" t="s">
+        <v>43</v>
+      </c>
       <c r="C11" s="8" t="s">
         <v>6</v>
       </c>
@@ -436,14 +766,17 @@
         <v>12</v>
       </c>
       <c r="E11" s="14">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="F11" s="11">
-        <v>2.18</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12">
+    <row r="12" spans="2:9" ht="15.6">
+      <c r="B12" s="33" t="s">
+        <v>43</v>
+      </c>
       <c r="C12" s="8" t="s">
         <v>6</v>
       </c>
@@ -451,7 +784,7 @@
         <v>13</v>
       </c>
       <c r="E12" s="14">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="F12" s="11">
         <v>1.82</v>
@@ -459,7 +792,10 @@
       <c r="H12" s="4"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13">
+    <row r="13" spans="2:9" ht="15">
+      <c r="B13" s="32" t="s">
+        <v>41</v>
+      </c>
       <c r="C13" s="8" t="s">
         <v>6</v>
       </c>
@@ -467,14 +803,17 @@
         <v>14</v>
       </c>
       <c r="E13" s="14">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="F13" s="11">
         <v>1.82</v>
       </c>
       <c r="H13" s="4"/>
     </row>
-    <row r="14">
+    <row r="14" spans="2:9" ht="15">
+      <c r="B14" s="32" t="s">
+        <v>41</v>
+      </c>
       <c r="C14" s="15" t="s">
         <v>15</v>
       </c>
@@ -482,7 +821,7 @@
         <v>16</v>
       </c>
       <c r="E14" s="17">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="F14" s="18">
         <v>5.91</v>
@@ -492,7 +831,10 @@
       </c>
       <c r="H14" s="4"/>
     </row>
-    <row r="15">
+    <row r="15" spans="2:9" ht="15">
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
       <c r="C15" s="15" t="s">
         <v>15</v>
       </c>
@@ -500,14 +842,17 @@
         <v>17</v>
       </c>
       <c r="E15" s="20">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="F15" s="18">
         <v>3.27</v>
       </c>
       <c r="H15" s="4"/>
     </row>
-    <row r="16">
+    <row r="16" spans="2:9" ht="15">
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
       <c r="C16" s="15" t="s">
         <v>15</v>
       </c>
@@ -515,7 +860,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="20">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="F16" s="18">
         <v>3.27</v>
@@ -523,7 +868,10 @@
       <c r="G16" s="3"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17">
+    <row r="17" spans="2:8" ht="15">
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
       <c r="C17" s="15" t="s">
         <v>15</v>
       </c>
@@ -531,14 +879,17 @@
         <v>19</v>
       </c>
       <c r="E17" s="20">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="F17" s="18">
         <v>3.18</v>
       </c>
       <c r="H17" s="4"/>
     </row>
-    <row r="18">
+    <row r="18" spans="2:8" ht="15">
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
       <c r="C18" s="15" t="s">
         <v>15</v>
       </c>
@@ -546,14 +897,17 @@
         <v>20</v>
       </c>
       <c r="E18" s="20">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="F18" s="18">
         <v>3.18</v>
       </c>
       <c r="H18" s="4"/>
     </row>
-    <row r="19">
+    <row r="19" spans="2:8" ht="15">
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
       <c r="C19" s="15" t="s">
         <v>15</v>
       </c>
@@ -561,14 +915,17 @@
         <v>21</v>
       </c>
       <c r="E19" s="20">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="F19" s="18">
         <v>3.18</v>
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20">
+    <row r="20" spans="2:8" ht="15">
+      <c r="B20" s="32" t="s">
+        <v>41</v>
+      </c>
       <c r="C20" s="15" t="s">
         <v>15</v>
       </c>
@@ -576,14 +933,17 @@
         <v>22</v>
       </c>
       <c r="E20" s="20">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="F20" s="18">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H20" s="4"/>
     </row>
-    <row r="21">
+    <row r="21" spans="2:8" ht="15">
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
       <c r="C21" s="15" t="s">
         <v>15</v>
       </c>
@@ -591,13 +951,16 @@
         <v>23</v>
       </c>
       <c r="E21" s="20">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="F21" s="18">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15">
+      <c r="B22" s="32" t="s">
+        <v>41</v>
+      </c>
       <c r="C22" s="15" t="s">
         <v>15</v>
       </c>
@@ -605,13 +968,16 @@
         <v>24</v>
       </c>
       <c r="E22" s="20">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="F22" s="18">
         <v>1.82</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="2:8" ht="15">
+      <c r="B23" s="32" t="s">
+        <v>41</v>
+      </c>
       <c r="C23" s="15" t="s">
         <v>15</v>
       </c>
@@ -619,13 +985,16 @@
         <v>25</v>
       </c>
       <c r="E23" s="20">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="F23" s="18">
         <v>1.27</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="2:8" ht="15">
+      <c r="B24" s="32" t="s">
+        <v>42</v>
+      </c>
       <c r="C24" s="15" t="s">
         <v>15</v>
       </c>
@@ -633,13 +1002,16 @@
         <v>26</v>
       </c>
       <c r="E24" s="20">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F24" s="18">
         <v>0.45</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="2:8" ht="15">
+      <c r="B25" s="32" t="s">
+        <v>41</v>
+      </c>
       <c r="C25" s="22" t="s">
         <v>27</v>
       </c>
@@ -648,13 +1020,16 @@
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="25">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="2:8" ht="15">
+      <c r="B26" s="33" t="s">
+        <v>43</v>
+      </c>
       <c r="C26" s="22" t="s">
         <v>27</v>
       </c>
@@ -663,10 +1038,13 @@
       </c>
       <c r="E26" s="24"/>
       <c r="F26" s="25">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="15">
+      <c r="B27" s="33" t="s">
+        <v>43</v>
+      </c>
       <c r="C27" s="26" t="s">
         <v>31</v>
       </c>
@@ -681,7 +1059,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="2:8" ht="15">
+      <c r="B28" s="33" t="s">
+        <v>43</v>
+      </c>
       <c r="C28" s="26" t="s">
         <v>31</v>
       </c>
@@ -693,7 +1074,10 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="2:8" ht="15">
+      <c r="B29" s="33" t="s">
+        <v>43</v>
+      </c>
       <c r="C29" s="26" t="s">
         <v>31</v>
       </c>
@@ -705,10 +1089,11 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="2:8" ht="15">
       <c r="D30" s="31"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Acabadas estructura de armas y actualizados estado de entregables del hito
</commit_message>
<xml_diff>
--- a/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
+++ b/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esgar\OneDrive\Documentos\Sack-3D\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Sack-3D\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -129,21 +129,6 @@
     <t>Armas</t>
   </si>
   <si>
-    <t>Movimiento, salto, hacerse el muerto y disparar</t>
-  </si>
-  <si>
-    <t>Cargador de mapas desde Tiled</t>
-  </si>
-  <si>
-    <t>Muelles y cosas</t>
-  </si>
-  <si>
-    <t>Moviento con los cubos creables</t>
-  </si>
-  <si>
-    <t>Coger y soltar cosas</t>
-  </si>
-  <si>
     <t>Falta esto</t>
   </si>
   <si>
@@ -151,6 +136,21 @@
   </si>
   <si>
     <t>Listo</t>
+  </si>
+  <si>
+    <t>(Falta volver a coger despues de muerto)</t>
+  </si>
+  <si>
+    <t>(Subir entregable con los 3 rayos)</t>
+  </si>
+  <si>
+    <t>Listo (usar otro entregable)</t>
+  </si>
+  <si>
+    <t>Ajustarlo</t>
+  </si>
+  <si>
+    <t>Cargador de (mas) mapas desde Tiled</t>
   </si>
 </sst>
 </file>
@@ -160,7 +160,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00;[Red]\-0.00;&quot;&quot;"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -216,6 +216,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -267,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -344,6 +350,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,18 +636,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I30"/>
+  <dimension ref="B2:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.21875" customWidth="1"/>
-    <col min="2" max="2" width="39.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="102.5546875" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="102.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="24.75" customHeight="1">
@@ -654,7 +661,7 @@
       <c r="G3" s="4"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="2:9" ht="15.6">
+    <row r="4" spans="2:9">
       <c r="D4" s="6" t="s">
         <v>1</v>
       </c>
@@ -662,11 +669,11 @@
       <c r="G4" s="4"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="2:9" ht="15.6">
+    <row r="5" spans="2:9">
       <c r="G5" s="4"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="2:9" ht="17.399999999999999">
+    <row r="6" spans="2:9" ht="18">
       <c r="C6" s="7" t="s">
         <v>2</v>
       </c>
@@ -681,9 +688,9 @@
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="2:9" ht="15.6">
+    <row r="7" spans="2:9">
       <c r="B7" s="32" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>6</v>
@@ -704,7 +711,7 @@
     </row>
     <row r="8" spans="2:9" ht="15">
       <c r="B8" s="32" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>6</v>
@@ -721,7 +728,7 @@
     </row>
     <row r="9" spans="2:9" ht="15">
       <c r="B9" s="32" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>6</v>
@@ -739,7 +746,7 @@
     </row>
     <row r="10" spans="2:9" ht="15">
       <c r="B10" s="33" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>6</v>
@@ -757,7 +764,7 @@
     </row>
     <row r="11" spans="2:9" ht="15">
       <c r="B11" s="33" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>6</v>
@@ -773,9 +780,9 @@
       </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="2:9" ht="15.6">
+    <row r="12" spans="2:9">
       <c r="B12" s="33" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>6</v>
@@ -794,7 +801,7 @@
     </row>
     <row r="13" spans="2:9" ht="15">
       <c r="B13" s="32" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>6</v>
@@ -812,7 +819,7 @@
     </row>
     <row r="14" spans="2:9" ht="15">
       <c r="B14" s="32" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>15</v>
@@ -832,8 +839,8 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="2:9" ht="15">
-      <c r="B15" t="s">
-        <v>39</v>
+      <c r="B15" s="33" t="s">
+        <v>38</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>15</v>
@@ -850,8 +857,8 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="2:9" ht="15">
-      <c r="B16" t="s">
-        <v>37</v>
+      <c r="B16" s="32" t="s">
+        <v>43</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>15</v>
@@ -869,7 +876,7 @@
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="2:8" ht="15">
-      <c r="B17" t="s">
+      <c r="B17" s="33" t="s">
         <v>38</v>
       </c>
       <c r="C17" s="15" t="s">
@@ -887,8 +894,8 @@
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="2:8" ht="15">
-      <c r="B18" t="s">
-        <v>36</v>
+      <c r="B18" s="32" t="s">
+        <v>39</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>15</v>
@@ -924,7 +931,7 @@
     </row>
     <row r="20" spans="2:8" ht="15">
       <c r="B20" s="32" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>15</v>
@@ -941,8 +948,8 @@
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="2:8" ht="15">
-      <c r="B21" t="s">
-        <v>40</v>
+      <c r="B21" s="33" t="s">
+        <v>41</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>15</v>
@@ -959,7 +966,7 @@
     </row>
     <row r="22" spans="2:8" ht="15">
       <c r="B22" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>15</v>
@@ -975,8 +982,8 @@
       </c>
     </row>
     <row r="23" spans="2:8" ht="15">
-      <c r="B23" s="32" t="s">
-        <v>41</v>
+      <c r="B23" s="33" t="s">
+        <v>38</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>15</v>
@@ -992,8 +999,8 @@
       </c>
     </row>
     <row r="24" spans="2:8" ht="15">
-      <c r="B24" s="32" t="s">
-        <v>42</v>
+      <c r="B24" s="34" t="s">
+        <v>37</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>15</v>
@@ -1010,7 +1017,7 @@
     </row>
     <row r="25" spans="2:8" ht="15">
       <c r="B25" s="32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>27</v>
@@ -1028,7 +1035,7 @@
     </row>
     <row r="26" spans="2:8" ht="15">
       <c r="B26" s="33" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>27</v>
@@ -1043,7 +1050,7 @@
     </row>
     <row r="27" spans="2:8" ht="15">
       <c r="B27" s="33" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>31</v>
@@ -1061,7 +1068,7 @@
     </row>
     <row r="28" spans="2:8" ht="15">
       <c r="B28" s="33" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>31</v>
@@ -1076,7 +1083,7 @@
     </row>
     <row r="29" spans="2:8" ht="15">
       <c r="B29" s="33" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C29" s="26" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Actualizado entregables hito uno.excel
</commit_message>
<xml_diff>
--- a/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
+++ b/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
   <si>
     <t>Lista de Entregables HITO 1</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>Boceto del entorno</t>
-  </si>
-  <si>
-    <t>Armas</t>
   </si>
   <si>
     <t>Falta esto</t>
@@ -639,7 +636,7 @@
   <dimension ref="B2:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -690,7 +687,7 @@
     </row>
     <row r="7" spans="2:9">
       <c r="B7" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>6</v>
@@ -711,7 +708,7 @@
     </row>
     <row r="8" spans="2:9" ht="15">
       <c r="B8" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>6</v>
@@ -728,7 +725,7 @@
     </row>
     <row r="9" spans="2:9" ht="15">
       <c r="B9" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>6</v>
@@ -746,7 +743,7 @@
     </row>
     <row r="10" spans="2:9" ht="15">
       <c r="B10" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>6</v>
@@ -764,7 +761,7 @@
     </row>
     <row r="11" spans="2:9" ht="15">
       <c r="B11" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>6</v>
@@ -782,7 +779,7 @@
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>6</v>
@@ -801,7 +798,7 @@
     </row>
     <row r="13" spans="2:9" ht="15">
       <c r="B13" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>6</v>
@@ -819,7 +816,7 @@
     </row>
     <row r="14" spans="2:9" ht="15">
       <c r="B14" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>15</v>
@@ -840,7 +837,7 @@
     </row>
     <row r="15" spans="2:9" ht="15">
       <c r="B15" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>15</v>
@@ -858,7 +855,7 @@
     </row>
     <row r="16" spans="2:9" ht="15">
       <c r="B16" s="32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>15</v>
@@ -877,7 +874,7 @@
     </row>
     <row r="17" spans="2:8" ht="15">
       <c r="B17" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>15</v>
@@ -895,7 +892,7 @@
     </row>
     <row r="18" spans="2:8" ht="15">
       <c r="B18" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>15</v>
@@ -912,8 +909,8 @@
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="2:8" ht="15">
-      <c r="B19" t="s">
-        <v>35</v>
+      <c r="B19" s="33" t="s">
+        <v>37</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>15</v>
@@ -931,7 +928,7 @@
     </row>
     <row r="20" spans="2:8" ht="15">
       <c r="B20" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>15</v>
@@ -949,7 +946,7 @@
     </row>
     <row r="21" spans="2:8" ht="15">
       <c r="B21" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>15</v>
@@ -966,7 +963,7 @@
     </row>
     <row r="22" spans="2:8" ht="15">
       <c r="B22" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>15</v>
@@ -983,7 +980,7 @@
     </row>
     <row r="23" spans="2:8" ht="15">
       <c r="B23" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>15</v>
@@ -1000,7 +997,7 @@
     </row>
     <row r="24" spans="2:8" ht="15">
       <c r="B24" s="34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>15</v>
@@ -1017,7 +1014,7 @@
     </row>
     <row r="25" spans="2:8" ht="15">
       <c r="B25" s="32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>27</v>
@@ -1035,7 +1032,7 @@
     </row>
     <row r="26" spans="2:8" ht="15">
       <c r="B26" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>27</v>
@@ -1050,7 +1047,7 @@
     </row>
     <row r="27" spans="2:8" ht="15">
       <c r="B27" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>31</v>
@@ -1068,7 +1065,7 @@
     </row>
     <row r="28" spans="2:8" ht="15">
       <c r="B28" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>31</v>
@@ -1083,7 +1080,7 @@
     </row>
     <row r="29" spans="2:8" ht="15">
       <c r="B29" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="26" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Cargador de 3 mapas funcional
</commit_message>
<xml_diff>
--- a/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
+++ b/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Sack-3D\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robeert\Documents\GitHub\ABP\Sack-3D\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
   <si>
     <t>Lista de Entregables HITO 1</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>Ajustarlo</t>
-  </si>
-  <si>
-    <t>Cargador de (mas) mapas desde Tiled</t>
   </si>
 </sst>
 </file>
@@ -636,7 +633,7 @@
   <dimension ref="B2:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -854,8 +851,8 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="2:9" ht="15">
-      <c r="B16" s="32" t="s">
-        <v>42</v>
+      <c r="B16" s="33" t="s">
+        <v>37</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Ajustado entregable mecanicas de acción y excel
</commit_message>
<xml_diff>
--- a/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
+++ b/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robeert\Documents\GitHub\ABP\Sack-3D\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Sack-3D\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
   <si>
     <t>Lista de Entregables HITO 1</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>Listo</t>
-  </si>
-  <si>
-    <t>(Falta volver a coger despues de muerto)</t>
   </si>
   <si>
     <t>(Subir entregable con los 3 rayos)</t>
@@ -633,7 +630,7 @@
   <dimension ref="B2:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -888,8 +885,8 @@
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="2:8" ht="15">
-      <c r="B18" s="32" t="s">
-        <v>38</v>
+      <c r="B18" s="33" t="s">
+        <v>37</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>15</v>
@@ -924,8 +921,8 @@
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="2:8" ht="15">
-      <c r="B20" s="32" t="s">
-        <v>35</v>
+      <c r="B20" s="33" t="s">
+        <v>37</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>15</v>
@@ -943,7 +940,7 @@
     </row>
     <row r="21" spans="2:8" ht="15">
       <c r="B21" s="33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>15</v>
@@ -960,7 +957,7 @@
     </row>
     <row r="22" spans="2:8" ht="15">
       <c r="B22" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>15</v>
@@ -1011,7 +1008,7 @@
     </row>
     <row r="25" spans="2:8" ht="15">
       <c r="B25" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Añadida division en fuente, ejecutable para entregables
</commit_message>
<xml_diff>
--- a/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
+++ b/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -630,7 +630,7 @@
   <dimension ref="B2:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Añadidas instrucciones a entregables y actualizado excel
</commit_message>
<xml_diff>
--- a/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
+++ b/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
@@ -141,7 +141,7 @@
     <t>Listo (usar otro entregable)</t>
   </si>
   <si>
-    <t>Ajustarlo</t>
+    <t>Hito 2 o 3</t>
   </si>
 </sst>
 </file>
@@ -629,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1007,8 +1007,8 @@
       </c>
     </row>
     <row r="25" spans="2:8" ht="15">
-      <c r="B25" s="32" t="s">
-        <v>40</v>
+      <c r="B25" s="33" t="s">
+        <v>37</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>27</v>
@@ -1026,7 +1026,7 @@
     </row>
     <row r="26" spans="2:8" ht="15">
       <c r="B26" s="33" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Añadido doc de red y actualizado excel
</commit_message>
<xml_diff>
--- a/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
+++ b/Documentacion/Lista_de_Entregables_Hito_Uno.xlsx
@@ -126,22 +126,22 @@
     <t>Boceto del entorno</t>
   </si>
   <si>
-    <t>Falta esto</t>
-  </si>
-  <si>
     <t>Esto no se ni que es</t>
   </si>
   <si>
     <t>Listo</t>
   </si>
   <si>
-    <t>(Subir entregable con los 3 rayos)</t>
-  </si>
-  <si>
     <t>Listo (usar otro entregable)</t>
   </si>
   <si>
     <t>Hito 2 o 3</t>
+  </si>
+  <si>
+    <t>Falta esto (pedir aplazarlo)</t>
+  </si>
+  <si>
+    <t>Listo (pobre)</t>
   </si>
 </sst>
 </file>
@@ -197,12 +197,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF21FF51"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -210,6 +204,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B0F0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -629,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -681,7 +681,7 @@
     </row>
     <row r="7" spans="2:9">
       <c r="B7" s="32" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>6</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="8" spans="2:9" ht="15">
       <c r="B8" s="32" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>6</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="9" spans="2:9" ht="15">
       <c r="B9" s="32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>6</v>
@@ -736,8 +736,8 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="2:9" ht="15">
-      <c r="B10" s="33" t="s">
-        <v>37</v>
+      <c r="B10" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>6</v>
@@ -754,8 +754,8 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="2:9" ht="15">
-      <c r="B11" s="33" t="s">
-        <v>37</v>
+      <c r="B11" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>6</v>
@@ -772,8 +772,8 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="33" t="s">
-        <v>37</v>
+      <c r="B12" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>6</v>
@@ -791,8 +791,8 @@
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="2:9" ht="15">
-      <c r="B13" s="32" t="s">
-        <v>35</v>
+      <c r="B13" s="34" t="s">
+        <v>39</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>6</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="14" spans="2:9" ht="15">
       <c r="B14" s="32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>15</v>
@@ -830,8 +830,8 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="2:9" ht="15">
-      <c r="B15" s="33" t="s">
-        <v>37</v>
+      <c r="B15" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>15</v>
@@ -848,8 +848,8 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="2:9" ht="15">
-      <c r="B16" s="33" t="s">
-        <v>37</v>
+      <c r="B16" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>15</v>
@@ -867,8 +867,8 @@
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="2:8" ht="15">
-      <c r="B17" s="33" t="s">
-        <v>37</v>
+      <c r="B17" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>15</v>
@@ -885,8 +885,8 @@
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="2:8" ht="15">
-      <c r="B18" s="33" t="s">
-        <v>37</v>
+      <c r="B18" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>15</v>
@@ -903,8 +903,8 @@
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="2:8" ht="15">
-      <c r="B19" s="33" t="s">
-        <v>37</v>
+      <c r="B19" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>15</v>
@@ -921,8 +921,8 @@
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="2:8" ht="15">
-      <c r="B20" s="33" t="s">
-        <v>37</v>
+      <c r="B20" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>15</v>
@@ -939,8 +939,8 @@
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="2:8" ht="15">
-      <c r="B21" s="33" t="s">
-        <v>39</v>
+      <c r="B21" s="32" t="s">
+        <v>37</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>15</v>
@@ -957,7 +957,7 @@
     </row>
     <row r="22" spans="2:8" ht="15">
       <c r="B22" s="32" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>15</v>
@@ -973,8 +973,8 @@
       </c>
     </row>
     <row r="23" spans="2:8" ht="15">
-      <c r="B23" s="33" t="s">
-        <v>37</v>
+      <c r="B23" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>15</v>
@@ -990,8 +990,8 @@
       </c>
     </row>
     <row r="24" spans="2:8" ht="15">
-      <c r="B24" s="34" t="s">
-        <v>36</v>
+      <c r="B24" s="33" t="s">
+        <v>35</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>15</v>
@@ -1007,8 +1007,8 @@
       </c>
     </row>
     <row r="25" spans="2:8" ht="15">
-      <c r="B25" s="33" t="s">
-        <v>37</v>
+      <c r="B25" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>27</v>
@@ -1025,8 +1025,8 @@
       </c>
     </row>
     <row r="26" spans="2:8" ht="15">
-      <c r="B26" s="33" t="s">
-        <v>40</v>
+      <c r="B26" s="32" t="s">
+        <v>38</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>27</v>
@@ -1040,8 +1040,8 @@
       </c>
     </row>
     <row r="27" spans="2:8" ht="15">
-      <c r="B27" s="33" t="s">
-        <v>37</v>
+      <c r="B27" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>31</v>
@@ -1058,8 +1058,8 @@
       </c>
     </row>
     <row r="28" spans="2:8" ht="15">
-      <c r="B28" s="33" t="s">
-        <v>37</v>
+      <c r="B28" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>31</v>
@@ -1073,8 +1073,8 @@
       </c>
     </row>
     <row r="29" spans="2:8" ht="15">
-      <c r="B29" s="33" t="s">
-        <v>37</v>
+      <c r="B29" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="C29" s="26" t="s">
         <v>31</v>

</xml_diff>